<commit_message>
Adding Fourth ICA for Lesson 01.3
</commit_message>
<xml_diff>
--- a/Lesson 01.3/StudentGrades_Solved.xlsx
+++ b/Lesson 01.3/StudentGrades_Solved.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ontextron-my.sharepoint.com/personal/khutula_txt_textron_com/Documents/Desktop/Class/in-class-activity-solutions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khutula\OneDrive - Textron\Desktop\Class\in-class-activity-solutions\Lesson 01.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{3B33A7F2-0661-4351-8EAC-300DCEA3A015}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-10125" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3730,7 +3730,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$4</c15:sqref>
@@ -3759,7 +3759,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
@@ -3791,7 +3791,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$4:$G$4</c15:sqref>
@@ -3823,7 +3823,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-077C-4D74-8D48-C098EABE3E91}"/>
                   </c:ext>
@@ -3836,7 +3836,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$5</c15:sqref>
@@ -3865,7 +3865,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
@@ -3897,7 +3897,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$5:$G$5</c15:sqref>
@@ -3929,7 +3929,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-077C-4D74-8D48-C098EABE3E91}"/>
                   </c:ext>
@@ -3942,7 +3942,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$6</c15:sqref>
@@ -3971,7 +3971,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
@@ -4003,7 +4003,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$6:$G$6</c15:sqref>
@@ -4035,7 +4035,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-077C-4D74-8D48-C098EABE3E91}"/>
                   </c:ext>
@@ -4048,7 +4048,7 @@
                 <c:order val="5"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$7</c15:sqref>
@@ -4077,7 +4077,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
@@ -4109,7 +4109,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$7:$G$7</c15:sqref>
@@ -4141,7 +4141,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-077C-4D74-8D48-C098EABE3E91}"/>
                   </c:ext>
@@ -4154,7 +4154,7 @@
                 <c:order val="6"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$8</c15:sqref>
@@ -4185,7 +4185,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
@@ -4217,7 +4217,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$8:$G$8</c15:sqref>
@@ -4249,7 +4249,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-077C-4D74-8D48-C098EABE3E91}"/>
                   </c:ext>
@@ -4262,7 +4262,7 @@
                 <c:order val="7"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$9</c15:sqref>
@@ -4293,7 +4293,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
@@ -4325,7 +4325,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$9:$G$9</c15:sqref>
@@ -4357,7 +4357,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-077C-4D74-8D48-C098EABE3E91}"/>
                   </c:ext>
@@ -4370,7 +4370,7 @@
                 <c:order val="8"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$10</c15:sqref>
@@ -4401,7 +4401,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
@@ -4433,7 +4433,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$10:$G$10</c15:sqref>
@@ -4465,7 +4465,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000008-077C-4D74-8D48-C098EABE3E91}"/>
                   </c:ext>
@@ -4478,7 +4478,7 @@
                 <c:order val="10"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$12</c15:sqref>
@@ -4509,7 +4509,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
@@ -4541,7 +4541,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$12:$G$12</c15:sqref>
@@ -4573,7 +4573,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000A-077C-4D74-8D48-C098EABE3E91}"/>
                   </c:ext>
@@ -4586,7 +4586,7 @@
                 <c:order val="11"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$13</c15:sqref>
@@ -4617,7 +4617,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
@@ -4649,7 +4649,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$13:$G$13</c15:sqref>
@@ -4681,7 +4681,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000B-077C-4D74-8D48-C098EABE3E91}"/>
                   </c:ext>
@@ -4694,7 +4694,7 @@
                 <c:order val="12"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$14</c15:sqref>
@@ -4726,7 +4726,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
@@ -4758,7 +4758,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$14:$G$14</c15:sqref>
@@ -4790,7 +4790,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000C-077C-4D74-8D48-C098EABE3E91}"/>
                   </c:ext>
@@ -4803,7 +4803,7 @@
                 <c:order val="13"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$15</c15:sqref>
@@ -4835,7 +4835,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
@@ -4867,7 +4867,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$15:$G$15</c15:sqref>
@@ -4899,7 +4899,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000D-077C-4D74-8D48-C098EABE3E91}"/>
                   </c:ext>
@@ -4912,7 +4912,7 @@
                 <c:order val="14"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$16</c15:sqref>
@@ -4944,7 +4944,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
@@ -4976,7 +4976,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$16:$G$16</c15:sqref>
@@ -5008,7 +5008,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000E-077C-4D74-8D48-C098EABE3E91}"/>
                   </c:ext>
@@ -5021,7 +5021,7 @@
                 <c:order val="15"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$17</c15:sqref>
@@ -5053,7 +5053,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
@@ -5085,7 +5085,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$17:$G$17</c15:sqref>
@@ -5117,7 +5117,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000F-077C-4D74-8D48-C098EABE3E91}"/>
                   </c:ext>
@@ -5130,7 +5130,7 @@
                 <c:order val="16"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$18</c15:sqref>
@@ -5162,7 +5162,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
@@ -5194,7 +5194,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$18:$G$18</c15:sqref>
@@ -5226,7 +5226,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000010-077C-4D74-8D48-C098EABE3E91}"/>
                   </c:ext>
@@ -5239,7 +5239,7 @@
                 <c:order val="17"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$19</c15:sqref>
@@ -5271,7 +5271,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
@@ -5303,7 +5303,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$19:$G$19</c15:sqref>
@@ -5335,7 +5335,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000011-077C-4D74-8D48-C098EABE3E91}"/>
                   </c:ext>
@@ -5348,7 +5348,7 @@
                 <c:order val="18"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$20</c15:sqref>
@@ -5379,7 +5379,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
@@ -5411,7 +5411,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$20:$G$20</c15:sqref>
@@ -5443,7 +5443,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000012-077C-4D74-8D48-C098EABE3E91}"/>
                   </c:ext>
@@ -5456,7 +5456,7 @@
                 <c:order val="19"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$21</c15:sqref>
@@ -5487,7 +5487,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$1:$G$1</c15:sqref>
@@ -5519,7 +5519,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$21:$G$21</c15:sqref>
@@ -5551,7 +5551,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000013-077C-4D74-8D48-C098EABE3E91}"/>
                   </c:ext>

</xml_diff>